<commit_message>
Aula17 FPOO, Excel e Javascript
</commit_message>
<xml_diff>
--- a/1des/sop/aula06/exercicios.xlsx
+++ b/1des/sop/aula06/exercicios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aula-c\senai\1des\sop\aula06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\aula-c\senai\1des\sop\aula06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A1932F-121A-4AD5-92B2-CE199BF651A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAFC1C4-5BCB-47A1-9738-D71A51C4892D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{9DAC40B0-2ADB-4978-A35B-B98804DC90B6}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
   <si>
     <t>Fases da Vida</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Rosiana</t>
+  </si>
+  <si>
+    <t>Salário Liq.</t>
   </si>
 </sst>
 </file>
@@ -204,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +231,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -249,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -258,6 +287,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,16 +610,16 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,19 +755,20 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -952,80 +988,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7B3C110-0401-4E5C-A92C-28BBBFBA1AD2}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="K1" s="5" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="L1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="6" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1033,199 +1073,215 @@
       <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="8">
         <v>1000</v>
       </c>
       <c r="C3" s="3">
-        <f>IF(B3&lt;=$H$3,B3*$I$3,IF(B3&lt;=$H$4,B3*$I$4,IF(B3&lt;=$H$5,B3*$I$5,IF(B3&lt;=$H$6,B3*$I$6,$H$6*$I$6))))</f>
+        <f>IF(B3&lt;=$I$3,B3*$J$3,IF(B3&lt;=$I$4,B3*$J$4,IF(B3&lt;=$I$5,B3*$J$5,IF(B3&lt;=$I$6,B3*$J$6,$I$6*$J$6))))</f>
         <v>75</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="8">
         <f>B3-C3</f>
         <v>925</v>
       </c>
       <c r="E3" s="4">
-        <f>IF(D3&lt;=$L$3, D3*$M$3-$N$3, IF(D3&lt;=$L$4, D3*$M$4-$N$4, IF(D3&lt;=$L$5, D3*$M$5-$N$5, IF(D3&lt;=$L$6, D3*$M$6-$N$6, D3*$M$7-$N$7))))</f>
+        <f>IF(D3&lt;=$M$3, D3*$N$3-$O$3, IF(D3&lt;=$M$4, D3*$N$4-$O$4, IF(D3&lt;=$M$5, D3*$N$5-$O$5, IF(D3&lt;=$M$6, D3*$N$6-$O$6, D3*$N$7-$O$7))))</f>
         <v>0</v>
       </c>
-      <c r="G3" s="3">
+      <c r="F3" s="8">
+        <f>D3-E3</f>
+        <v>925</v>
+      </c>
+      <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="8">
         <v>1320</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="8">
         <v>2112</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="8">
         <v>0</v>
       </c>
-      <c r="O3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="8">
         <v>2000</v>
       </c>
       <c r="C4" s="3">
-        <f t="shared" ref="C4:C11" si="0">IF(B4&lt;=$H$3,B4*$I$3,IF(B4&lt;=$H$4,B4*$I$4,IF(B4&lt;=$H$5,B4*$I$5,IF(B4&lt;=$H$6,B4*$I$6,$H$6*$I$6))))</f>
+        <f>IF(B4&lt;=$I$3,B4*$J$3,IF(B4&lt;=$I$4,B4*$J$4,IF(B4&lt;=$I$5,B4*$J$5,IF(B4&lt;=$I$6,B4*$J$6,$I$6*$J$6))))</f>
         <v>180</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="8">
         <f>B4-C4</f>
         <v>1820</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E11" si="1">IF(D4&lt;=$L$3, D4*$M$3-$N$3, IF(D4&lt;=$L$4, D4*$M$4-$N$4, IF(D4&lt;=$L$5, D4*$M$5-$N$5, IF(D4&lt;=$L$6, D4*$M$6-$N$6, D4*$M$7-$N$7))))</f>
+        <f>IF(D4&lt;=$M$3, D4*$N$3-$O$3, IF(D4&lt;=$M$4, D4*$N$4-$O$4, IF(D4&lt;=$M$5, D4*$N$5-$O$5, IF(D4&lt;=$M$6, D4*$N$6-$O$6, D4*$N$7-$O$7))))</f>
         <v>0</v>
       </c>
-      <c r="G4" s="3">
+      <c r="F4" s="8">
+        <f t="shared" ref="F4:F11" si="0">D4-E4</f>
+        <v>1820</v>
+      </c>
+      <c r="H4" s="3">
         <v>1320.01</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="8">
         <v>2571.29</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.09</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>2112.0100000000002</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="8">
         <v>2826.65</v>
       </c>
-      <c r="M4" s="2">
+      <c r="N4" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="8">
         <v>158.4</v>
       </c>
-      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="8">
         <v>3000</v>
       </c>
       <c r="C5" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B5&lt;=$I$3,B5*$J$3,IF(B5&lt;=$I$4,B5*$J$4,IF(B5&lt;=$I$5,B5*$J$5,IF(B5&lt;=$I$6,B5*$J$6,$I$6*$J$6))))</f>
         <v>360</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="8">
         <f>B5-C5</f>
         <v>2640</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D5&lt;=$M$3, D5*$N$3-$O$3, IF(D5&lt;=$M$4, D5*$N$4-$O$4, IF(D5&lt;=$M$5, D5*$N$5-$O$5, IF(D5&lt;=$M$6, D5*$N$6-$O$6, D5*$N$7-$O$7))))</f>
         <v>39.599999999999994</v>
       </c>
-      <c r="G5" s="3">
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>2600.4</v>
+      </c>
+      <c r="H5" s="3">
         <v>2571.3000000000002</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="8">
         <v>3856.94</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <v>0.12</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>2826.66</v>
       </c>
-      <c r="L5" s="3">
+      <c r="M5" s="8">
         <v>3751.06</v>
       </c>
-      <c r="M5" s="2">
+      <c r="N5" s="2">
         <v>0.15</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="8">
         <v>370.4</v>
       </c>
-      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="8">
         <v>4000</v>
       </c>
       <c r="C6" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B6&lt;=$I$3,B6*$J$3,IF(B6&lt;=$I$4,B6*$J$4,IF(B6&lt;=$I$5,B6*$J$5,IF(B6&lt;=$I$6,B6*$J$6,$I$6*$J$6))))</f>
         <v>560</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="8">
         <f>B6-C6</f>
         <v>3440</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D6&lt;=$M$3, D6*$N$3-$O$3, IF(D6&lt;=$M$4, D6*$N$4-$O$4, IF(D6&lt;=$M$5, D6*$N$5-$O$5, IF(D6&lt;=$M$6, D6*$N$6-$O$6, D6*$N$7-$O$7))))</f>
         <v>145.60000000000002</v>
       </c>
-      <c r="G6" s="3">
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>3294.4</v>
+      </c>
+      <c r="H6" s="3">
         <v>3856.95</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="8">
         <v>7507.49</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L6" s="3">
         <v>3751.07</v>
       </c>
-      <c r="L6" s="3">
+      <c r="M6" s="8">
         <v>4664.68</v>
       </c>
-      <c r="M6" s="2">
+      <c r="N6" s="2">
         <v>0.22500000000000001</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="8">
         <v>651.73</v>
       </c>
-      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="8">
         <v>5000</v>
       </c>
       <c r="C7" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B7&lt;=$I$3,B7*$J$3,IF(B7&lt;=$I$4,B7*$J$4,IF(B7&lt;=$I$5,B7*$J$5,IF(B7&lt;=$I$6,B7*$J$6,$I$6*$J$6))))</f>
         <v>700.00000000000011</v>
       </c>
-      <c r="D7" s="3">
-        <f t="shared" ref="D4:D11" si="2">B7-C7</f>
+      <c r="D7" s="8">
+        <f t="shared" ref="D7:E11" si="1">B7-C7</f>
         <v>4300</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D7&lt;=$M$3, D7*$N$3-$O$3, IF(D7&lt;=$M$4, D7*$N$4-$O$4, IF(D7&lt;=$M$5, D7*$N$5-$O$5, IF(D7&lt;=$M$6, D7*$N$6-$O$6, D7*$N$7-$O$7))))</f>
         <v>315.77</v>
       </c>
-      <c r="K7" t="s">
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>3984.23</v>
+      </c>
+      <c r="L7" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="8">
         <v>0</v>
       </c>
-      <c r="M7" s="2">
+      <c r="N7" s="2">
         <v>0.27500000000000002</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="8">
         <v>884.96</v>
       </c>
     </row>
@@ -1233,87 +1289,106 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="8">
         <v>6000</v>
       </c>
       <c r="C8" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B8&lt;=$I$3,B8*$J$3,IF(B8&lt;=$I$4,B8*$J$4,IF(B8&lt;=$I$5,B8*$J$5,IF(B8&lt;=$I$6,B8*$J$6,$I$6*$J$6))))</f>
         <v>840.00000000000011</v>
       </c>
-      <c r="D8" s="3">
-        <f t="shared" si="2"/>
+      <c r="D8" s="8">
+        <f t="shared" si="1"/>
         <v>5160</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D8&lt;=$M$3, D8*$N$3-$O$3, IF(D8&lt;=$M$4, D8*$N$4-$O$4, IF(D8&lt;=$M$5, D8*$N$5-$O$5, IF(D8&lt;=$M$6, D8*$N$6-$O$6, D8*$N$7-$O$7))))</f>
         <v>534.04000000000019</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>4625.96</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="8">
         <v>7000</v>
       </c>
       <c r="C9" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B9&lt;=$I$3,B9*$J$3,IF(B9&lt;=$I$4,B9*$J$4,IF(B9&lt;=$I$5,B9*$J$5,IF(B9&lt;=$I$6,B9*$J$6,$I$6*$J$6))))</f>
         <v>980.00000000000011</v>
       </c>
-      <c r="D9" s="3">
-        <f t="shared" si="2"/>
+      <c r="D9" s="8">
+        <f t="shared" si="1"/>
         <v>6020</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D9&lt;=$M$3, D9*$N$3-$O$3, IF(D9&lt;=$M$4, D9*$N$4-$O$4, IF(D9&lt;=$M$5, D9*$N$5-$O$5, IF(D9&lt;=$M$6, D9*$N$6-$O$6, D9*$N$7-$O$7))))</f>
         <v>770.54000000000019</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>5249.46</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="8">
         <v>8000</v>
       </c>
       <c r="C10" s="3">
-        <f>IF(B10&lt;=$H$3,B10*$I$3,IF(B10&lt;=$H$4,B10*$I$4,IF(B10&lt;=$H$5,B10*$I$5,IF(B10&lt;=$H$6,B10*$I$6,$H$6*$I$6))))</f>
+        <f>IF(B10&lt;=$I$3,B10*$J$3,IF(B10&lt;=$I$4,B10*$J$4,IF(B10&lt;=$I$5,B10*$J$5,IF(B10&lt;=$I$6,B10*$J$6,$I$6*$J$6))))</f>
         <v>1051.0486000000001</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" si="2"/>
+      <c r="D10" s="8">
+        <f t="shared" si="1"/>
         <v>6948.9513999999999</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D10&lt;=$M$3, D10*$N$3-$O$3, IF(D10&lt;=$M$4, D10*$N$4-$O$4, IF(D10&lt;=$M$5, D10*$N$5-$O$5, IF(D10&lt;=$M$6, D10*$N$6-$O$6, D10*$N$7-$O$7))))</f>
         <v>1026.0016350000001</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>5922.9497649999994</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="17.25" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="8">
         <v>10000</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" si="0"/>
+        <f>IF(B11&lt;=$I$3,B11*$J$3,IF(B11&lt;=$I$4,B11*$J$4,IF(B11&lt;=$I$5,B11*$J$5,IF(B11&lt;=$I$6,B11*$J$6,$I$6*$J$6))))</f>
         <v>1051.0486000000001</v>
       </c>
-      <c r="D11" s="3">
-        <f t="shared" si="2"/>
+      <c r="D11" s="8">
+        <f t="shared" si="1"/>
         <v>8948.9513999999999</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="1"/>
+        <f>IF(D11&lt;=$M$3, D11*$N$3-$O$3, IF(D11&lt;=$M$4, D11*$N$4-$O$4, IF(D11&lt;=$M$5, D11*$N$5-$O$5, IF(D11&lt;=$M$6, D11*$N$6-$O$6, D11*$N$7-$O$7))))</f>
         <v>1576.0016350000001</v>
       </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>7372.9497649999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>